<commit_message>
change in ticl_import module
</commit_message>
<xml_diff>
--- a/ticl_import/sample_file/update_recycled_date.xlsx
+++ b/ticl_import/sample_file/update_recycled_date.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">Unique</t>
   </si>
@@ -31,25 +31,19 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">1036</t>
+    <t xml:space="preserve">9042</t>
   </si>
   <si>
     <t xml:space="preserve">test gsdg</t>
   </si>
   <si>
-    <t xml:space="preserve">1035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1015</t>
+    <t xml:space="preserve">9035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9001</t>
   </si>
   <si>
     <t xml:space="preserve">test gsdg testttttttttt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test gsdgdfbfdbvdf dsv</t>
   </si>
 </sst>
 </file>
@@ -183,10 +177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,17 +243,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>45064</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>